<commit_message>
Update / harmonize column naming
</commit_message>
<xml_diff>
--- a/inputs/Columns.xlsx
+++ b/inputs/Columns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\DR_mod\DR_Potentials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DR_mod\DR_Potentials\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194E5DE4-22FE-4729-B76C-3FBA282A4647}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77097C60-D397-491E-AA11-22E734E90FC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="448">
   <si>
     <t>Gruppe</t>
   </si>
@@ -1316,6 +1316,54 @@
   </si>
   <si>
     <t>nein</t>
+  </si>
+  <si>
+    <t>Potenzial pos. MW Tag 15 min</t>
+  </si>
+  <si>
+    <t>Potenzial pos. MW Tag 2 h</t>
+  </si>
+  <si>
+    <t>Potenzial pos. MW Tag 30 min</t>
+  </si>
+  <si>
+    <t>Potenzial pos. MW Tag 4 h</t>
+  </si>
+  <si>
+    <t>Potenzial pos. MW Nacht 15 min</t>
+  </si>
+  <si>
+    <t>Potenzial pos. MW Nacht 2 h</t>
+  </si>
+  <si>
+    <t>Potenzial pos. MW Nacht 30 min</t>
+  </si>
+  <si>
+    <t>Potenzial pos. MW Nacht 4 h</t>
+  </si>
+  <si>
+    <t>Potenzial neg. MW Nacht 15 min</t>
+  </si>
+  <si>
+    <t>Potenzial neg. MW Nacht 2 h</t>
+  </si>
+  <si>
+    <t>Potenzial neg. MW Nacht 30 min</t>
+  </si>
+  <si>
+    <t>Potenzial neg. MW Nacht 4 h</t>
+  </si>
+  <si>
+    <t>Potenzial neg. MW Tag 15 min</t>
+  </si>
+  <si>
+    <t>Potenzial neg. MW Tag 2 h</t>
+  </si>
+  <si>
+    <t>Potenzial neg. MW Tag 30 min</t>
+  </si>
+  <si>
+    <t>Potenzial neg. MW Tag 4 h</t>
   </si>
 </sst>
 </file>
@@ -1517,8 +1565,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D07D76C7-2024-4812-A583-9AEA703D99BF}" name="Tabelle2" displayName="Tabelle2" ref="A1:E392" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E392" xr:uid="{5E9F0B9F-2BE9-4EAB-99B9-EE5EE1F96A82}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D07D76C7-2024-4812-A583-9AEA703D99BF}" name="Tabelle2" displayName="Tabelle2" ref="A1:E408" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E408" xr:uid="{5E9F0B9F-2BE9-4EAB-99B9-EE5EE1F96A82}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{354C2B9C-026C-4A8E-BFA8-A99211BC8AE4}" name="Spaltenname" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{2971FB75-8976-49B2-8AA0-40D58A8C0143}" name="Gruppe" dataDxfId="3"/>
@@ -1851,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E392"/>
+  <dimension ref="A1:E408"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
+      <selection activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4299,7 +4347,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>138</v>
+        <v>440</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>397</v>
@@ -4316,7 +4364,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>139</v>
+        <v>441</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>397</v>
@@ -4333,7 +4381,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>140</v>
+        <v>442</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>397</v>
@@ -4350,7 +4398,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>141</v>
+        <v>443</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>397</v>
@@ -4367,7 +4415,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>397</v>
@@ -4384,7 +4432,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>397</v>
@@ -4401,10 +4449,10 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>430</v>
@@ -4418,10 +4466,10 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>145</v>
+        <v>444</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>430</v>
@@ -4435,10 +4483,10 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>146</v>
+        <v>445</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>430</v>
@@ -4452,10 +4500,10 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>147</v>
+        <v>446</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>430</v>
@@ -4469,10 +4517,10 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>148</v>
+        <v>447</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>430</v>
@@ -4486,10 +4534,10 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>430</v>
@@ -4503,10 +4551,10 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>430</v>
@@ -4520,10 +4568,10 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>430</v>
@@ -4537,7 +4585,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B158" s="2" t="s">
         <v>407</v>
@@ -4554,10 +4602,10 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>430</v>
@@ -4571,10 +4619,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>430</v>
@@ -4588,10 +4636,10 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>430</v>
@@ -4605,10 +4653,10 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>430</v>
@@ -4622,10 +4670,10 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>430</v>
@@ -4639,10 +4687,10 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>430</v>
@@ -4656,10 +4704,10 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>430</v>
@@ -4673,10 +4721,10 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>430</v>
@@ -4690,7 +4738,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B167" s="2" t="s">
         <v>408</v>
@@ -4707,10 +4755,10 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>430</v>
@@ -4724,10 +4772,10 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>430</v>
@@ -4741,10 +4789,10 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>430</v>
@@ -4758,10 +4806,10 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>430</v>
@@ -4775,10 +4823,10 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>430</v>
@@ -4792,10 +4840,10 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>389</v>
+        <v>408</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>430</v>
@@ -4809,10 +4857,10 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>430</v>
@@ -4826,10 +4874,10 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>430</v>
@@ -4843,10 +4891,10 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>430</v>
@@ -4860,10 +4908,10 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>430</v>
@@ -4877,10 +4925,10 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>430</v>
@@ -4894,10 +4942,10 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>430</v>
@@ -4911,10 +4959,10 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>430</v>
@@ -4928,16 +4976,16 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>423</v>
@@ -4945,10 +4993,10 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>430</v>
@@ -4962,10 +5010,10 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>430</v>
@@ -4979,10 +5027,10 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>430</v>
@@ -4996,16 +5044,16 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>423</v>
@@ -5013,10 +5061,10 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>430</v>
@@ -5030,10 +5078,10 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>430</v>
@@ -5047,10 +5095,10 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>430</v>
@@ -5064,10 +5112,10 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>430</v>
@@ -5081,7 +5129,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>398</v>
@@ -5098,16 +5146,16 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E191" s="3" t="s">
         <v>423</v>
@@ -5115,7 +5163,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>398</v>
@@ -5132,10 +5180,10 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>430</v>
@@ -5149,7 +5197,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>398</v>
@@ -5166,7 +5214,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>398</v>
@@ -5183,16 +5231,16 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C196" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>423</v>
@@ -5200,16 +5248,16 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>398</v>
+        <v>414</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>423</v>
@@ -5217,16 +5265,16 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>423</v>
@@ -5234,16 +5282,16 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>398</v>
+        <v>414</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>423</v>
@@ -5251,16 +5299,16 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>423</v>
@@ -5268,16 +5316,16 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>398</v>
+        <v>415</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>423</v>
@@ -5285,16 +5333,16 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>196</v>
+        <v>436</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>423</v>
@@ -5302,7 +5350,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>197</v>
+        <v>437</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>398</v>
@@ -5319,16 +5367,16 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>198</v>
+        <v>438</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>423</v>
@@ -5336,10 +5384,10 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>199</v>
+        <v>439</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>430</v>
@@ -5353,10 +5401,10 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>430</v>
@@ -5370,16 +5418,16 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>423</v>
@@ -5387,16 +5435,16 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>423</v>
@@ -5404,16 +5452,16 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C209" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>423</v>
@@ -5421,16 +5469,16 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>423</v>
@@ -5438,16 +5486,16 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>205</v>
+        <v>432</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E211" s="3" t="s">
         <v>423</v>
@@ -5455,10 +5503,10 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>206</v>
+        <v>433</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>430</v>
@@ -5472,16 +5520,16 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>207</v>
+        <v>434</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E213" s="3" t="s">
         <v>423</v>
@@ -5489,10 +5537,10 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>208</v>
+        <v>435</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>430</v>
@@ -5506,16 +5554,16 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>423</v>
@@ -5523,16 +5571,16 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C216" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E216" s="3" t="s">
         <v>423</v>
@@ -5540,16 +5588,16 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C217" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E217" s="3" t="s">
         <v>423</v>
@@ -5557,16 +5605,16 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C218" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E218" s="3" t="s">
         <v>423</v>
@@ -5574,16 +5622,16 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>415</v>
+        <v>398</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E219" s="3" t="s">
         <v>423</v>
@@ -5591,16 +5639,16 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E220" s="3" t="s">
         <v>423</v>
@@ -5608,16 +5656,16 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C221" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E221" s="3" t="s">
         <v>423</v>
@@ -5625,10 +5673,10 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>430</v>
@@ -5642,16 +5690,16 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>423</v>
@@ -5659,16 +5707,16 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C224" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>423</v>
@@ -5676,16 +5724,16 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E225" s="3" t="s">
         <v>423</v>
@@ -5693,16 +5741,16 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C226" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E226" s="3" t="s">
         <v>423</v>
@@ -5710,16 +5758,16 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="C227" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>423</v>
@@ -5727,16 +5775,16 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C228" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E228" s="3" t="s">
         <v>423</v>
@@ -5744,16 +5792,16 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="C229" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>423</v>
@@ -5761,16 +5809,16 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E230" s="3" t="s">
         <v>423</v>
@@ -5778,16 +5826,16 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="C231" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E231" s="3" t="s">
         <v>423</v>
@@ -5795,16 +5843,16 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>423</v>
@@ -5812,16 +5860,16 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E233" s="3" t="s">
         <v>423</v>
@@ -5829,16 +5877,16 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E234" s="3" t="s">
         <v>423</v>
@@ -5846,16 +5894,16 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E235" s="3" t="s">
         <v>423</v>
@@ -5863,16 +5911,16 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E236" s="3" t="s">
         <v>423</v>
@@ -5880,16 +5928,16 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E237" s="3" t="s">
         <v>423</v>
@@ -5897,16 +5945,16 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="C238" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E238" s="3" t="s">
         <v>423</v>
@@ -5914,10 +5962,10 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>430</v>
@@ -5931,7 +5979,7 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="B240" s="2" t="s">
         <v>416</v>
@@ -5948,10 +5996,10 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>430</v>
@@ -5965,7 +6013,7 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="B242" s="2" t="s">
         <v>416</v>
@@ -5982,10 +6030,10 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="C243" s="2" t="s">
         <v>430</v>
@@ -5999,7 +6047,7 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>416</v>
@@ -6016,10 +6064,10 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="C245" s="2" t="s">
         <v>430</v>
@@ -6033,16 +6081,16 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>398</v>
+        <v>416</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D246" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E246" s="3" t="s">
         <v>423</v>
@@ -6050,10 +6098,10 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>389</v>
+        <v>410</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>430</v>
@@ -6067,16 +6115,16 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D248" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E248" s="3" t="s">
         <v>423</v>
@@ -6084,10 +6132,10 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C249" s="2" t="s">
         <v>430</v>
@@ -6101,10 +6149,10 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="C250" s="2" t="s">
         <v>430</v>
@@ -6118,10 +6166,10 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C251" s="2" t="s">
         <v>430</v>
@@ -6135,16 +6183,16 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="C252" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D252" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E252" s="3" t="s">
         <v>423</v>
@@ -6152,16 +6200,16 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C253" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D253" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E253" s="3" t="s">
         <v>423</v>
@@ -6169,16 +6217,16 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="C254" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D254" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E254" s="3" t="s">
         <v>423</v>
@@ -6186,10 +6234,10 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="C255" s="2" t="s">
         <v>430</v>
@@ -6203,16 +6251,16 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="C256" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D256" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E256" s="3" t="s">
         <v>423</v>
@@ -6220,16 +6268,16 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="C257" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D257" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E257" s="3" t="s">
         <v>423</v>
@@ -6237,16 +6285,16 @@
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D258" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E258" s="3" t="s">
         <v>423</v>
@@ -6254,95 +6302,95 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B259" s="1" t="s">
-        <v>253</v>
+        <v>237</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>398</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D259" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E259" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E259" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>399</v>
+        <v>416</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D260" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E260" s="2" t="s">
-        <v>422</v>
+        <v>418</v>
+      </c>
+      <c r="E260" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D261" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E261" s="2" t="s">
-        <v>422</v>
+        <v>417</v>
+      </c>
+      <c r="E261" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C262" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D262" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E262" s="2" t="s">
-        <v>422</v>
+        <v>417</v>
+      </c>
+      <c r="E262" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C263" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E263" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E263" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C264" s="2" t="s">
         <v>430</v>
@@ -6351,15 +6399,15 @@
         <v>417</v>
       </c>
       <c r="E264" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C265" s="2" t="s">
         <v>430</v>
@@ -6368,32 +6416,32 @@
         <v>417</v>
       </c>
       <c r="E265" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C266" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E266" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="C267" s="2" t="s">
         <v>430</v>
@@ -6402,66 +6450,66 @@
         <v>417</v>
       </c>
       <c r="E267" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E268" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>400</v>
+        <v>415</v>
       </c>
       <c r="C269" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E269" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="C270" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E270" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="C271" s="2" t="s">
         <v>430</v>
@@ -6470,55 +6518,55 @@
         <v>417</v>
       </c>
       <c r="E271" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="C272" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E272" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B273" s="1" t="s">
-        <v>267</v>
+        <v>251</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>416</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D273" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E273" s="2" t="s">
-        <v>426</v>
+        <v>418</v>
+      </c>
+      <c r="E273" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="C274" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D274" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E274" s="3" t="s">
         <v>423</v>
@@ -6526,27 +6574,27 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B275" s="2" t="s">
-        <v>401</v>
+        <v>253</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D275" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E275" s="3" t="s">
-        <v>423</v>
+      <c r="E275" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C276" s="2" t="s">
         <v>430</v>
@@ -6554,16 +6602,16 @@
       <c r="D276" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E276" s="3" t="s">
-        <v>423</v>
+      <c r="E276" s="2" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C277" s="2" t="s">
         <v>430</v>
@@ -6571,16 +6619,16 @@
       <c r="D277" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E277" s="3" t="s">
-        <v>423</v>
+      <c r="E277" s="2" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C278" s="2" t="s">
         <v>430</v>
@@ -6588,16 +6636,16 @@
       <c r="D278" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E278" s="3" t="s">
-        <v>423</v>
+      <c r="E278" s="2" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="C279" s="2" t="s">
         <v>430</v>
@@ -6605,67 +6653,67 @@
       <c r="D279" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E279" s="3" t="s">
-        <v>423</v>
+      <c r="E279" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>389</v>
+        <v>411</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D280" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E280" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E280" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>389</v>
+        <v>411</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E281" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E281" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>389</v>
+        <v>411</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E282" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E282" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C283" s="2" t="s">
         <v>430</v>
@@ -6679,16 +6727,16 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>402</v>
+        <v>419</v>
       </c>
       <c r="C284" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E284" s="3" t="s">
         <v>422</v>
@@ -6696,10 +6744,10 @@
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C285" s="2" t="s">
         <v>430</v>
@@ -6713,16 +6761,16 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>402</v>
+        <v>419</v>
       </c>
       <c r="C286" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D286" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E286" s="3" t="s">
         <v>422</v>
@@ -6730,10 +6778,10 @@
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C287" s="2" t="s">
         <v>430</v>
@@ -6747,16 +6795,16 @@
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>402</v>
+        <v>419</v>
       </c>
       <c r="C288" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E288" s="3" t="s">
         <v>422</v>
@@ -6764,95 +6812,95 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B289" s="2" t="s">
-        <v>402</v>
+        <v>267</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E289" s="3" t="s">
-        <v>422</v>
+        <v>428</v>
+      </c>
+      <c r="E289" s="2" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C290" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E290" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C291" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E291" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C292" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E292" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="C293" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E293" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="C294" s="2" t="s">
         <v>430</v>
@@ -6861,15 +6909,15 @@
         <v>428</v>
       </c>
       <c r="E294" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="C295" s="2" t="s">
         <v>430</v>
@@ -6878,72 +6926,72 @@
         <v>428</v>
       </c>
       <c r="E295" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D296" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E296" s="3" t="s">
-        <v>422</v>
+      <c r="E296" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D297" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E297" s="3" t="s">
-        <v>422</v>
+      <c r="E297" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D298" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E298" s="3" t="s">
-        <v>422</v>
+      <c r="E298" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C299" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E299" s="3" t="s">
         <v>422</v>
@@ -6951,16 +6999,16 @@
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C300" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E300" s="3" t="s">
         <v>422</v>
@@ -6968,16 +7016,16 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C301" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E301" s="3" t="s">
         <v>422</v>
@@ -6985,50 +7033,50 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E302" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E302" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="C303" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E303" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="C304" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E304" s="3" t="s">
         <v>422</v>
@@ -7036,16 +7084,16 @@
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="C305" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E305" s="3" t="s">
         <v>422</v>
@@ -7053,16 +7101,16 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="C306" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E306" s="3" t="s">
         <v>422</v>
@@ -7070,16 +7118,16 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="C307" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D307" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E307" s="3" t="s">
         <v>422</v>
@@ -7087,16 +7135,16 @@
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E308" s="3" t="s">
         <v>422</v>
@@ -7104,7 +7152,7 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="B309" s="2" t="s">
         <v>389</v>
@@ -7113,7 +7161,7 @@
         <v>430</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E309" s="3" t="s">
         <v>422</v>
@@ -7121,7 +7169,7 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="B310" s="2" t="s">
         <v>391</v>
@@ -7138,27 +7186,27 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C311" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D311" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E311" s="2" t="s">
-        <v>424</v>
+      <c r="E311" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>430</v>
@@ -7172,10 +7220,10 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="C313" s="2" t="s">
         <v>430</v>
@@ -7189,10 +7237,10 @@
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="C314" s="2" t="s">
         <v>430</v>
@@ -7206,10 +7254,10 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>430</v>
@@ -7223,10 +7271,10 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>430</v>
@@ -7240,10 +7288,10 @@
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>390</v>
+        <v>403</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>430</v>
@@ -7257,27 +7305,27 @@
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D318" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E318" s="3" t="s">
-        <v>422</v>
+      <c r="E318" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>430</v>
@@ -7286,15 +7334,15 @@
         <v>428</v>
       </c>
       <c r="E319" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>430</v>
@@ -7308,10 +7356,10 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C321" s="2" t="s">
         <v>430</v>
@@ -7325,10 +7373,10 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C322" s="2" t="s">
         <v>430</v>
@@ -7342,10 +7390,10 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C323" s="2" t="s">
         <v>430</v>
@@ -7359,10 +7407,10 @@
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C324" s="2" t="s">
         <v>430</v>
@@ -7376,10 +7424,10 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C325" s="2" t="s">
         <v>430</v>
@@ -7393,10 +7441,10 @@
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="C326" s="2" t="s">
         <v>430</v>
@@ -7410,27 +7458,27 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D327" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E327" s="3" t="s">
-        <v>422</v>
+      <c r="E327" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="C328" s="2" t="s">
         <v>430</v>
@@ -7444,10 +7492,10 @@
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="C329" s="2" t="s">
         <v>430</v>
@@ -7461,10 +7509,10 @@
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="C330" s="2" t="s">
         <v>430</v>
@@ -7478,10 +7526,10 @@
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="C331" s="2" t="s">
         <v>430</v>
@@ -7495,10 +7543,10 @@
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="C332" s="2" t="s">
         <v>430</v>
@@ -7507,15 +7555,15 @@
         <v>428</v>
       </c>
       <c r="E332" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="C333" s="2" t="s">
         <v>430</v>
@@ -7524,15 +7572,15 @@
         <v>428</v>
       </c>
       <c r="E333" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="C334" s="2" t="s">
         <v>430</v>
@@ -7541,15 +7589,15 @@
         <v>428</v>
       </c>
       <c r="E334" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C335" s="2" t="s">
         <v>430</v>
@@ -7558,15 +7606,15 @@
         <v>428</v>
       </c>
       <c r="E335" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C336" s="2" t="s">
         <v>430</v>
@@ -7575,15 +7623,15 @@
         <v>428</v>
       </c>
       <c r="E336" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C337" s="2" t="s">
         <v>430</v>
@@ -7592,15 +7640,15 @@
         <v>428</v>
       </c>
       <c r="E337" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="C338" s="2" t="s">
         <v>430</v>
@@ -7609,15 +7657,15 @@
         <v>428</v>
       </c>
       <c r="E338" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="C339" s="2" t="s">
         <v>430</v>
@@ -7626,15 +7674,15 @@
         <v>428</v>
       </c>
       <c r="E339" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="C340" s="2" t="s">
         <v>430</v>
@@ -7643,15 +7691,15 @@
         <v>428</v>
       </c>
       <c r="E340" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="C341" s="2" t="s">
         <v>430</v>
@@ -7660,21 +7708,21 @@
         <v>428</v>
       </c>
       <c r="E341" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C342" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D342" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E342" s="3" t="s">
         <v>422</v>
@@ -7682,16 +7730,16 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="C343" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D343" s="2" t="s">
-        <v>108</v>
+        <v>428</v>
       </c>
       <c r="E343" s="3" t="s">
         <v>422</v>
@@ -7699,16 +7747,16 @@
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C344" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D344" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E344" s="3" t="s">
         <v>422</v>
@@ -7716,16 +7764,16 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="C345" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D345" s="2" t="s">
-        <v>108</v>
+        <v>428</v>
       </c>
       <c r="E345" s="3" t="s">
         <v>422</v>
@@ -7733,16 +7781,16 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C346" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D346" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E346" s="3" t="s">
         <v>422</v>
@@ -7750,16 +7798,16 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C347" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D347" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E347" s="3" t="s">
         <v>422</v>
@@ -7767,180 +7815,180 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="C348" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D348" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="E348" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C349" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D349" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E349" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D350" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E350" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="B351" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D351" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E351" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="C352" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D352" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="E352" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D353" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="E353" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>420</v>
+        <v>389</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D354" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="E354" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="B355" s="2" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D355" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E355" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D356" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E356" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="B357" s="2" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D357" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E357" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>430</v>
@@ -7954,16 +8002,16 @@
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>412</v>
+        <v>420</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D359" s="2" t="s">
-        <v>417</v>
+        <v>108</v>
       </c>
       <c r="E359" s="3" t="s">
         <v>422</v>
@@ -7971,16 +8019,16 @@
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>393</v>
+        <v>406</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D360" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E360" s="3" t="s">
         <v>422</v>
@@ -7988,16 +8036,16 @@
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="B361" s="2" t="s">
-        <v>393</v>
+        <v>420</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D361" s="2" t="s">
-        <v>428</v>
+        <v>108</v>
       </c>
       <c r="E361" s="3" t="s">
         <v>422</v>
@@ -8005,101 +8053,101 @@
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D362" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E362" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="B363" s="2" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D363" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E363" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>389</v>
+        <v>420</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D364" s="2" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="E364" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="B365" s="2" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D365" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E365" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="B366" s="2" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="C366" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D366" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E366" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="B367" s="2" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D367" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E367" s="3" t="s">
         <v>422</v>
@@ -8107,16 +8155,16 @@
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="B368" s="2" t="s">
-        <v>389</v>
+        <v>420</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D368" s="2" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="E368" s="3" t="s">
         <v>422</v>
@@ -8124,16 +8172,16 @@
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="B369" s="2" t="s">
-        <v>389</v>
+        <v>420</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D369" s="2" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="E369" s="3" t="s">
         <v>422</v>
@@ -8141,16 +8189,16 @@
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="B370" s="2" t="s">
-        <v>389</v>
+        <v>420</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D370" s="2" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="E370" s="3" t="s">
         <v>422</v>
@@ -8158,16 +8206,16 @@
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="B371" s="2" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E371" s="3" t="s">
         <v>422</v>
@@ -8175,27 +8223,27 @@
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="B372" s="2" t="s">
-        <v>389</v>
+        <v>406</v>
       </c>
       <c r="C372" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D372" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E372" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E372" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="B373" s="2" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>430</v>
@@ -8209,10 +8257,10 @@
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>388</v>
+        <v>412</v>
       </c>
       <c r="C374" s="2" t="s">
         <v>430</v>
@@ -8226,10 +8274,10 @@
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="B375" s="2" t="s">
-        <v>388</v>
+        <v>412</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>430</v>
@@ -8243,16 +8291,16 @@
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="C376" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D376" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="E376" s="3" t="s">
         <v>422</v>
@@ -8260,16 +8308,16 @@
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="E377" s="3" t="s">
         <v>422</v>
@@ -8277,101 +8325,101 @@
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D378" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="E378" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D379" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E379" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D380" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="E380" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C381" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D381" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E381" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C382" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D382" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E382" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="B383" s="2" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="C383" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D383" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="E383" s="3" t="s">
         <v>422</v>
@@ -8379,16 +8427,16 @@
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="B384" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C384" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D384" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E384" s="3" t="s">
         <v>422</v>
@@ -8396,16 +8444,16 @@
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="B385" s="2" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="C385" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D385" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="E385" s="3" t="s">
         <v>422</v>
@@ -8413,16 +8461,16 @@
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="B386" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C386" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D386" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E386" s="3" t="s">
         <v>422</v>
@@ -8430,16 +8478,16 @@
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="B387" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C387" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D387" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E387" s="3" t="s">
         <v>422</v>
@@ -8447,67 +8495,67 @@
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C388" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D388" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E388" s="3" t="s">
-        <v>422</v>
+        <v>428</v>
+      </c>
+      <c r="E388" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C389" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D389" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E389" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E389" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C390" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D390" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E390" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E390" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C391" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D391" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E391" s="3" t="s">
         <v>422</v>
@@ -8515,18 +8563,290 @@
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B392" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C392" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D392" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E392" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A393" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B393" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C393" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D393" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E393" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A394" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B394" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C394" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D394" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E394" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A395" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B395" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C395" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D395" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E395" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A396" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B396" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C396" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D396" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E396" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A397" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B397" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C397" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D397" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E397" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A398" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B398" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C398" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D398" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E398" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A399" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B399" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C399" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D399" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E399" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A400" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B400" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C400" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D400" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E400" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A401" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B401" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C401" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D401" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E401" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A402" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B402" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C402" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D402" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E402" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A403" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B403" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C403" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D403" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E403" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A404" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B404" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C404" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D404" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E404" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A405" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B405" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C405" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D405" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E405" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A406" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B406" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C406" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D406" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E406" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A407" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B407" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C407" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D407" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E407" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A408" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B392" s="2" t="s">
+      <c r="B408" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="C392" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D392" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E392" s="3" t="s">
+      <c r="C408" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D408" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E408" s="3" t="s">
         <v>422</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add potential values and newly introduced column
</commit_message>
<xml_diff>
--- a/inputs/Columns.xlsx
+++ b/inputs/Columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DR_mod\DR_Potentials\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77097C60-D397-491E-AA11-22E734E90FC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDA6820-527E-4DF8-8FB5-28490DE4BABB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="449">
   <si>
     <t>Gruppe</t>
   </si>
@@ -1364,6 +1364,9 @@
   </si>
   <si>
     <t>Potenzial neg. MW Tag 4 h</t>
+  </si>
+  <si>
+    <t>Stromverbrauch in TWh errechnet</t>
   </si>
 </sst>
 </file>
@@ -1565,8 +1568,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D07D76C7-2024-4812-A583-9AEA703D99BF}" name="Tabelle2" displayName="Tabelle2" ref="A1:E408" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E408" xr:uid="{5E9F0B9F-2BE9-4EAB-99B9-EE5EE1F96A82}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D07D76C7-2024-4812-A583-9AEA703D99BF}" name="Tabelle2" displayName="Tabelle2" ref="A1:E409" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E409" xr:uid="{5E9F0B9F-2BE9-4EAB-99B9-EE5EE1F96A82}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{354C2B9C-026C-4A8E-BFA8-A99211BC8AE4}" name="Spaltenname" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{2971FB75-8976-49B2-8AA0-40D58A8C0143}" name="Gruppe" dataDxfId="3"/>
@@ -1899,10 +1902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E408"/>
+  <dimension ref="A1:E409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
-      <selection activeCell="E155" sqref="E155"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6863,7 +6866,7 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>270</v>
+        <v>448</v>
       </c>
       <c r="B292" s="2" t="s">
         <v>401</v>
@@ -6880,7 +6883,7 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>401</v>
@@ -6897,7 +6900,7 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B294" s="2" t="s">
         <v>401</v>
@@ -6914,7 +6917,7 @@
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>401</v>
@@ -6931,24 +6934,24 @@
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D296" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E296" s="2" t="s">
-        <v>424</v>
+      <c r="E296" s="3" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B297" s="2" t="s">
         <v>389</v>
@@ -6965,7 +6968,7 @@
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B298" s="2" t="s">
         <v>389</v>
@@ -6982,24 +6985,24 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E299" s="3" t="s">
-        <v>422</v>
+        <v>428</v>
+      </c>
+      <c r="E299" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>402</v>
@@ -7016,7 +7019,7 @@
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>402</v>
@@ -7033,7 +7036,7 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>402</v>
@@ -7050,7 +7053,7 @@
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B303" s="2" t="s">
         <v>402</v>
@@ -7067,7 +7070,7 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>402</v>
@@ -7084,7 +7087,7 @@
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B305" s="2" t="s">
         <v>402</v>
@@ -7101,7 +7104,7 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B306" s="2" t="s">
         <v>402</v>
@@ -7118,7 +7121,7 @@
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B307" s="2" t="s">
         <v>402</v>
@@ -7135,7 +7138,7 @@
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B308" s="2" t="s">
         <v>402</v>
@@ -7152,10 +7155,10 @@
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>389</v>
+        <v>402</v>
       </c>
       <c r="C309" s="2" t="s">
         <v>430</v>
@@ -7169,16 +7172,16 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E310" s="3" t="s">
         <v>422</v>
@@ -7186,7 +7189,7 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B311" s="2" t="s">
         <v>391</v>
@@ -7203,7 +7206,7 @@
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B312" s="2" t="s">
         <v>391</v>
@@ -7220,10 +7223,10 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="C313" s="2" t="s">
         <v>430</v>
@@ -7237,7 +7240,7 @@
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B314" s="2" t="s">
         <v>403</v>
@@ -7254,7 +7257,7 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B315" s="2" t="s">
         <v>403</v>
@@ -7271,7 +7274,7 @@
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B316" s="2" t="s">
         <v>403</v>
@@ -7288,7 +7291,7 @@
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B317" s="2" t="s">
         <v>403</v>
@@ -7305,44 +7308,44 @@
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D318" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E318" s="2" t="s">
-        <v>424</v>
+      <c r="E318" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D319" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E319" s="3" t="s">
-        <v>423</v>
+      <c r="E319" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>430</v>
@@ -7351,12 +7354,12 @@
         <v>428</v>
       </c>
       <c r="E320" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>389</v>
@@ -7373,7 +7376,7 @@
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B322" s="2" t="s">
         <v>389</v>
@@ -7390,7 +7393,7 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B323" s="2" t="s">
         <v>389</v>
@@ -7407,7 +7410,7 @@
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B324" s="2" t="s">
         <v>389</v>
@@ -7424,7 +7427,7 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B325" s="2" t="s">
         <v>389</v>
@@ -7441,10 +7444,10 @@
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C326" s="2" t="s">
         <v>430</v>
@@ -7458,41 +7461,41 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C327" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D327" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E327" s="2" t="s">
-        <v>424</v>
+      <c r="E327" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C328" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D328" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E328" s="3" t="s">
-        <v>422</v>
+      <c r="E328" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B329" s="2" t="s">
         <v>390</v>
@@ -7509,7 +7512,7 @@
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B330" s="2" t="s">
         <v>390</v>
@@ -7526,7 +7529,7 @@
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B331" s="2" t="s">
         <v>390</v>
@@ -7543,7 +7546,7 @@
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B332" s="2" t="s">
         <v>390</v>
@@ -7560,7 +7563,7 @@
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B333" s="2" t="s">
         <v>390</v>
@@ -7577,7 +7580,7 @@
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B334" s="2" t="s">
         <v>390</v>
@@ -7594,10 +7597,10 @@
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="C335" s="2" t="s">
         <v>430</v>
@@ -7611,7 +7614,7 @@
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B336" s="2" t="s">
         <v>404</v>
@@ -7628,7 +7631,7 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B337" s="2" t="s">
         <v>404</v>
@@ -7645,7 +7648,7 @@
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>404</v>
@@ -7662,7 +7665,7 @@
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B339" s="2" t="s">
         <v>404</v>
@@ -7679,7 +7682,7 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B340" s="2" t="s">
         <v>404</v>
@@ -7696,7 +7699,7 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B341" s="2" t="s">
         <v>404</v>
@@ -7713,7 +7716,7 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B342" s="2" t="s">
         <v>404</v>
@@ -7730,7 +7733,7 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B343" s="2" t="s">
         <v>404</v>
@@ -7747,7 +7750,7 @@
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B344" s="2" t="s">
         <v>404</v>
@@ -7764,7 +7767,7 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B345" s="2" t="s">
         <v>404</v>
@@ -7781,7 +7784,7 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B346" s="2" t="s">
         <v>404</v>
@@ -7798,7 +7801,7 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B347" s="2" t="s">
         <v>404</v>
@@ -7815,10 +7818,10 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C348" s="2" t="s">
         <v>430</v>
@@ -7827,12 +7830,12 @@
         <v>428</v>
       </c>
       <c r="E348" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B349" s="2" t="s">
         <v>405</v>
@@ -7849,7 +7852,7 @@
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B350" s="2" t="s">
         <v>405</v>
@@ -7866,7 +7869,7 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B351" s="2" t="s">
         <v>405</v>
@@ -7883,7 +7886,7 @@
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B352" s="2" t="s">
         <v>405</v>
@@ -7900,7 +7903,7 @@
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B353" s="2" t="s">
         <v>405</v>
@@ -7917,10 +7920,10 @@
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>430</v>
@@ -7934,7 +7937,7 @@
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B355" s="2" t="s">
         <v>389</v>
@@ -7951,7 +7954,7 @@
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B356" s="2" t="s">
         <v>389</v>
@@ -7968,7 +7971,7 @@
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B357" s="2" t="s">
         <v>389</v>
@@ -7985,33 +7988,33 @@
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D358" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E358" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D359" s="2" t="s">
-        <v>108</v>
+        <v>417</v>
       </c>
       <c r="E359" s="3" t="s">
         <v>422</v>
@@ -8019,16 +8022,16 @@
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D360" s="2" t="s">
-        <v>417</v>
+        <v>108</v>
       </c>
       <c r="E360" s="3" t="s">
         <v>422</v>
@@ -8036,16 +8039,16 @@
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B361" s="2" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="C361" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D361" s="2" t="s">
-        <v>108</v>
+        <v>417</v>
       </c>
       <c r="E361" s="3" t="s">
         <v>422</v>
@@ -8053,16 +8056,16 @@
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D362" s="2" t="s">
-        <v>417</v>
+        <v>108</v>
       </c>
       <c r="E362" s="3" t="s">
         <v>422</v>
@@ -8070,7 +8073,7 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B363" s="2" t="s">
         <v>406</v>
@@ -8087,16 +8090,16 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D364" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E364" s="3" t="s">
         <v>422</v>
@@ -8104,16 +8107,16 @@
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B365" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D365" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E365" s="3" t="s">
         <v>422</v>
@@ -8121,7 +8124,7 @@
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B366" s="2" t="s">
         <v>406</v>
@@ -8138,7 +8141,7 @@
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B367" s="2" t="s">
         <v>406</v>
@@ -8155,16 +8158,16 @@
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B368" s="2" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="C368" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D368" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E368" s="3" t="s">
         <v>422</v>
@@ -8172,7 +8175,7 @@
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B369" s="2" t="s">
         <v>420</v>
@@ -8189,7 +8192,7 @@
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B370" s="2" t="s">
         <v>420</v>
@@ -8206,16 +8209,16 @@
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B371" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C371" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D371" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E371" s="3" t="s">
         <v>422</v>
@@ -8223,7 +8226,7 @@
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B372" s="2" t="s">
         <v>406</v>
@@ -8240,7 +8243,7 @@
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B373" s="2" t="s">
         <v>406</v>
@@ -8257,10 +8260,10 @@
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="C374" s="2" t="s">
         <v>430</v>
@@ -8274,7 +8277,7 @@
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B375" s="2" t="s">
         <v>412</v>
@@ -8291,16 +8294,16 @@
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>393</v>
+        <v>412</v>
       </c>
       <c r="C376" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D376" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E376" s="3" t="s">
         <v>422</v>
@@ -8308,7 +8311,7 @@
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B377" s="2" t="s">
         <v>393</v>
@@ -8325,10 +8328,10 @@
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>430</v>
@@ -8337,12 +8340,12 @@
         <v>428</v>
       </c>
       <c r="E378" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B379" s="2" t="s">
         <v>389</v>
@@ -8359,7 +8362,7 @@
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B380" s="2" t="s">
         <v>389</v>
@@ -8376,7 +8379,7 @@
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B381" s="2" t="s">
         <v>389</v>
@@ -8393,7 +8396,7 @@
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B382" s="2" t="s">
         <v>389</v>
@@ -8410,7 +8413,7 @@
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B383" s="2" t="s">
         <v>389</v>
@@ -8422,12 +8425,12 @@
         <v>428</v>
       </c>
       <c r="E383" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B384" s="2" t="s">
         <v>389</v>
@@ -8444,7 +8447,7 @@
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B385" s="2" t="s">
         <v>389</v>
@@ -8461,7 +8464,7 @@
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B386" s="2" t="s">
         <v>389</v>
@@ -8478,7 +8481,7 @@
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B387" s="2" t="s">
         <v>389</v>
@@ -8495,41 +8498,41 @@
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B388" s="2" t="s">
         <v>389</v>
       </c>
       <c r="C388" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D388" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E388" s="2" t="s">
-        <v>424</v>
+      <c r="E388" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C389" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D389" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E389" s="3" t="s">
-        <v>422</v>
+        <v>428</v>
+      </c>
+      <c r="E389" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B390" s="2" t="s">
         <v>388</v>
@@ -8546,7 +8549,7 @@
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B391" s="2" t="s">
         <v>388</v>
@@ -8563,16 +8566,16 @@
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="C392" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D392" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E392" s="3" t="s">
         <v>422</v>
@@ -8580,7 +8583,7 @@
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B393" s="2" t="s">
         <v>413</v>
@@ -8597,7 +8600,7 @@
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B394" s="2" t="s">
         <v>413</v>
@@ -8614,16 +8617,16 @@
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="C395" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D395" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E395" s="3" t="s">
         <v>422</v>
@@ -8631,16 +8634,16 @@
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D396" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E396" s="3" t="s">
         <v>422</v>
@@ -8648,16 +8651,16 @@
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B397" s="2" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D397" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E397" s="3" t="s">
         <v>422</v>
@@ -8665,7 +8668,7 @@
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B398" s="2" t="s">
         <v>388</v>
@@ -8682,16 +8685,16 @@
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B399" s="2" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="C399" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D399" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E399" s="3" t="s">
         <v>422</v>
@@ -8699,16 +8702,16 @@
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="C400" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D400" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E400" s="3" t="s">
         <v>422</v>
@@ -8716,16 +8719,16 @@
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="C401" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D401" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E401" s="3" t="s">
         <v>422</v>
@@ -8733,16 +8736,16 @@
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="C402" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D402" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E402" s="3" t="s">
         <v>422</v>
@@ -8750,7 +8753,7 @@
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B403" s="2" t="s">
         <v>388</v>
@@ -8767,7 +8770,7 @@
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B404" s="2" t="s">
         <v>388</v>
@@ -8784,24 +8787,24 @@
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B405" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C405" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D405" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E405" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E405" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B406" s="2" t="s">
         <v>389</v>
@@ -8818,24 +8821,24 @@
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B407" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C407" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D407" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E407" s="3" t="s">
-        <v>422</v>
+      <c r="E407" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B408" s="2" t="s">
         <v>390</v>
@@ -8847,6 +8850,23 @@
         <v>428</v>
       </c>
       <c r="E408" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A409" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B409" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C409" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D409" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E409" s="3" t="s">
         <v>422</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update list of possible columns
</commit_message>
<xml_diff>
--- a/inputs/Columns.xlsx
+++ b/inputs/Columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DR_mod\DR_Potentials\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDA6820-527E-4DF8-8FB5-28490DE4BABB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0622D5-C8F9-4BBA-92B9-87B795546681}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="451">
   <si>
     <t>Gruppe</t>
   </si>
@@ -1367,6 +1367,12 @@
   </si>
   <si>
     <t>Stromverbrauch in TWh errechnet</t>
+  </si>
+  <si>
+    <t>flexibilisierbarer Anteil Lastreduktion</t>
+  </si>
+  <si>
+    <t>flexibilisierbarer Anteil Lastverzicht</t>
   </si>
 </sst>
 </file>
@@ -1568,8 +1574,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D07D76C7-2024-4812-A583-9AEA703D99BF}" name="Tabelle2" displayName="Tabelle2" ref="A1:E409" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E409" xr:uid="{5E9F0B9F-2BE9-4EAB-99B9-EE5EE1F96A82}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D07D76C7-2024-4812-A583-9AEA703D99BF}" name="Tabelle2" displayName="Tabelle2" ref="A1:E411" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E411" xr:uid="{5E9F0B9F-2BE9-4EAB-99B9-EE5EE1F96A82}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{354C2B9C-026C-4A8E-BFA8-A99211BC8AE4}" name="Spaltenname" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{2971FB75-8976-49B2-8AA0-40D58A8C0143}" name="Gruppe" dataDxfId="3"/>
@@ -1902,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E409"/>
+  <dimension ref="A1:E411"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7665,7 +7671,7 @@
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
-        <v>316</v>
+        <v>449</v>
       </c>
       <c r="B339" s="2" t="s">
         <v>404</v>
@@ -7674,7 +7680,7 @@
         <v>430</v>
       </c>
       <c r="D339" s="2" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="E339" s="3" t="s">
         <v>422</v>
@@ -7682,7 +7688,7 @@
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
-        <v>317</v>
+        <v>450</v>
       </c>
       <c r="B340" s="2" t="s">
         <v>404</v>
@@ -7691,7 +7697,7 @@
         <v>430</v>
       </c>
       <c r="D340" s="2" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="E340" s="3" t="s">
         <v>422</v>
@@ -7699,7 +7705,7 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B341" s="2" t="s">
         <v>404</v>
@@ -7716,7 +7722,7 @@
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B342" s="2" t="s">
         <v>404</v>
@@ -7733,7 +7739,7 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B343" s="2" t="s">
         <v>404</v>
@@ -7750,7 +7756,7 @@
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B344" s="2" t="s">
         <v>404</v>
@@ -7767,7 +7773,7 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B345" s="2" t="s">
         <v>404</v>
@@ -7784,7 +7790,7 @@
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B346" s="2" t="s">
         <v>404</v>
@@ -7801,7 +7807,7 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B347" s="2" t="s">
         <v>404</v>
@@ -7818,7 +7824,7 @@
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B348" s="2" t="s">
         <v>404</v>
@@ -7835,10 +7841,10 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C349" s="2" t="s">
         <v>430</v>
@@ -7847,15 +7853,15 @@
         <v>428</v>
       </c>
       <c r="E349" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>430</v>
@@ -7864,12 +7870,12 @@
         <v>428</v>
       </c>
       <c r="E350" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B351" s="2" t="s">
         <v>405</v>
@@ -7886,7 +7892,7 @@
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B352" s="2" t="s">
         <v>405</v>
@@ -7903,7 +7909,7 @@
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B353" s="2" t="s">
         <v>405</v>
@@ -7920,7 +7926,7 @@
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B354" s="2" t="s">
         <v>405</v>
@@ -7937,10 +7943,10 @@
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B355" s="2" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>430</v>
@@ -7954,10 +7960,10 @@
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>430</v>
@@ -7971,7 +7977,7 @@
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B357" s="2" t="s">
         <v>389</v>
@@ -7988,7 +7994,7 @@
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B358" s="2" t="s">
         <v>389</v>
@@ -8005,41 +8011,41 @@
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="C359" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D359" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E359" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>420</v>
+        <v>389</v>
       </c>
       <c r="C360" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D360" s="2" t="s">
-        <v>108</v>
+        <v>428</v>
       </c>
       <c r="E360" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B361" s="2" t="s">
         <v>406</v>
@@ -8056,7 +8062,7 @@
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B362" s="2" t="s">
         <v>420</v>
@@ -8073,7 +8079,7 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B363" s="2" t="s">
         <v>406</v>
@@ -8090,16 +8096,16 @@
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D364" s="2" t="s">
-        <v>417</v>
+        <v>108</v>
       </c>
       <c r="E364" s="3" t="s">
         <v>422</v>
@@ -8107,16 +8113,16 @@
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B365" s="2" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="C365" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D365" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E365" s="3" t="s">
         <v>422</v>
@@ -8124,7 +8130,7 @@
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B366" s="2" t="s">
         <v>406</v>
@@ -8141,16 +8147,16 @@
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B367" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C367" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D367" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E367" s="3" t="s">
         <v>422</v>
@@ -8158,7 +8164,7 @@
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B368" s="2" t="s">
         <v>406</v>
@@ -8175,16 +8181,16 @@
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B369" s="2" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="C369" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D369" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E369" s="3" t="s">
         <v>422</v>
@@ -8192,16 +8198,16 @@
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B370" s="2" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="C370" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D370" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E370" s="3" t="s">
         <v>422</v>
@@ -8209,7 +8215,7 @@
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B371" s="2" t="s">
         <v>420</v>
@@ -8226,16 +8232,16 @@
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B372" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C372" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D372" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E372" s="3" t="s">
         <v>422</v>
@@ -8243,16 +8249,16 @@
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B373" s="2" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="C373" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D373" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E373" s="3" t="s">
         <v>422</v>
@@ -8260,7 +8266,7 @@
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B374" s="2" t="s">
         <v>406</v>
@@ -8277,10 +8283,10 @@
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B375" s="2" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="C375" s="2" t="s">
         <v>430</v>
@@ -8294,10 +8300,10 @@
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="C376" s="2" t="s">
         <v>430</v>
@@ -8311,16 +8317,16 @@
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>393</v>
+        <v>412</v>
       </c>
       <c r="C377" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D377" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E377" s="3" t="s">
         <v>422</v>
@@ -8328,16 +8334,16 @@
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>393</v>
+        <v>412</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D378" s="2" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E378" s="3" t="s">
         <v>422</v>
@@ -8345,10 +8351,10 @@
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="C379" s="2" t="s">
         <v>430</v>
@@ -8357,15 +8363,15 @@
         <v>428</v>
       </c>
       <c r="E379" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="C380" s="2" t="s">
         <v>430</v>
@@ -8374,12 +8380,12 @@
         <v>428</v>
       </c>
       <c r="E380" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B381" s="2" t="s">
         <v>389</v>
@@ -8396,7 +8402,7 @@
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B382" s="2" t="s">
         <v>389</v>
@@ -8413,7 +8419,7 @@
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B383" s="2" t="s">
         <v>389</v>
@@ -8430,7 +8436,7 @@
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B384" s="2" t="s">
         <v>389</v>
@@ -8442,12 +8448,12 @@
         <v>428</v>
       </c>
       <c r="E384" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B385" s="2" t="s">
         <v>389</v>
@@ -8459,12 +8465,12 @@
         <v>428</v>
       </c>
       <c r="E385" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B386" s="2" t="s">
         <v>389</v>
@@ -8481,7 +8487,7 @@
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B387" s="2" t="s">
         <v>389</v>
@@ -8498,7 +8504,7 @@
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B388" s="2" t="s">
         <v>389</v>
@@ -8515,33 +8521,33 @@
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B389" s="2" t="s">
         <v>389</v>
       </c>
       <c r="C389" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D389" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E389" s="2" t="s">
-        <v>424</v>
+      <c r="E389" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C390" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D390" s="2" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="E390" s="3" t="s">
         <v>422</v>
@@ -8549,24 +8555,24 @@
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C391" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D391" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E391" s="3" t="s">
-        <v>422</v>
+        <v>428</v>
+      </c>
+      <c r="E391" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B392" s="2" t="s">
         <v>388</v>
@@ -8583,16 +8589,16 @@
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="C393" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D393" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E393" s="3" t="s">
         <v>422</v>
@@ -8600,16 +8606,16 @@
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="C394" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D394" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E394" s="3" t="s">
         <v>422</v>
@@ -8617,7 +8623,7 @@
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B395" s="2" t="s">
         <v>413</v>
@@ -8634,16 +8640,16 @@
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D396" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E396" s="3" t="s">
         <v>422</v>
@@ -8651,7 +8657,7 @@
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B397" s="2" t="s">
         <v>413</v>
@@ -8668,7 +8674,7 @@
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B398" s="2" t="s">
         <v>388</v>
@@ -8685,16 +8691,16 @@
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B399" s="2" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="C399" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D399" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E399" s="3" t="s">
         <v>422</v>
@@ -8702,16 +8708,16 @@
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="C400" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D400" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E400" s="3" t="s">
         <v>422</v>
@@ -8719,7 +8725,7 @@
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B401" s="2" t="s">
         <v>388</v>
@@ -8736,7 +8742,7 @@
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B402" s="2" t="s">
         <v>413</v>
@@ -8753,7 +8759,7 @@
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B403" s="2" t="s">
         <v>388</v>
@@ -8770,16 +8776,16 @@
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>388</v>
+        <v>413</v>
       </c>
       <c r="C404" s="2" t="s">
         <v>430</v>
       </c>
       <c r="D404" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E404" s="3" t="s">
         <v>422</v>
@@ -8787,7 +8793,7 @@
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B405" s="2" t="s">
         <v>388</v>
@@ -8804,69 +8810,103 @@
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C406" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D406" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E406" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E406" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B407" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C407" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D407" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E407" s="2" t="s">
-        <v>424</v>
+        <v>417</v>
+      </c>
+      <c r="E407" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B408" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C408" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D408" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="E408" s="3" t="s">
-        <v>422</v>
+      <c r="E408" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B409" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C409" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D409" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E409" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A410" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B410" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C410" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D410" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E410" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A411" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="B409" s="2" t="s">
+      <c r="B411" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="C409" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D409" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E409" s="3" t="s">
+      <c r="C411" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D411" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E411" s="3" t="s">
         <v>422</v>
       </c>
     </row>

</xml_diff>